<commit_message>
Add floor and delete site functionality
</commit_message>
<xml_diff>
--- a/template2.xlsx
+++ b/template2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbekmezian/Documents/mycode/projects/DNAC_Utility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F6541B7-2584-4641-8042-6253DF509BE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A4ECDC-A04A-074F-8E0D-BBF51B30DF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="860" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{2DCD80CE-93A4-A048-BA4F-5B1599A40A02}"/>
+    <workbookView xWindow="3960" yWindow="1540" windowWidth="26840" windowHeight="15940" xr2:uid="{2DCD80CE-93A4-A048-BA4F-5B1599A40A02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>Level</t>
   </si>
@@ -54,42 +54,15 @@
     <t>area</t>
   </si>
   <si>
-    <t>L1 Area 1</t>
-  </si>
-  <si>
     <t>building</t>
   </si>
   <si>
-    <t>13971 Ivie Farms Dr, Herriman, UT, 84096</t>
-  </si>
-  <si>
-    <t>L1 Area 1/L2 Area 1</t>
-  </si>
-  <si>
-    <t>L1 Area 1/L2 Area 1/L3 Area 1</t>
-  </si>
-  <si>
     <t>L1 Area 1/L2 Area 1/L3 Area 1/L3 Building 1</t>
   </si>
   <si>
-    <t>L1 Area 2</t>
-  </si>
-  <si>
-    <t>L1 Area 2/L2 Area 2</t>
-  </si>
-  <si>
-    <t>L1 Area 2/L2 Area 2/L3 Area 2</t>
-  </si>
-  <si>
     <t>L1 Area 2/L2 Area 2/L3 Area 2/L3 Building 1</t>
   </si>
   <si>
-    <t>L1 Area 3</t>
-  </si>
-  <si>
-    <t>13951 Ivie Farms Dr, Herriman, UT, 84096</t>
-  </si>
-  <si>
     <t>Pool Name</t>
   </si>
   <si>
@@ -148,6 +121,84 @@
   </si>
   <si>
     <t>POOL_Area1_Building1_CORP_VN_BMS</t>
+  </si>
+  <si>
+    <t>Floor Type (Cubes And Walled Offices, Drywall Office Only, Indoor High Ceiling, Outdoor Open Space)</t>
+  </si>
+  <si>
+    <t>Width
+(Floor only)</t>
+  </si>
+  <si>
+    <t>Length
+(Floor only)</t>
+  </si>
+  <si>
+    <t>Heigth
+(Floor only)</t>
+  </si>
+  <si>
+    <t>Americas</t>
+  </si>
+  <si>
+    <t>Americas/USBC</t>
+  </si>
+  <si>
+    <t>Americas/USBC/Building 1</t>
+  </si>
+  <si>
+    <t>9131 North Lake View St., Prior Lake, MN 55372</t>
+  </si>
+  <si>
+    <t>Americas/USBC/Building 1/Floor 1</t>
+  </si>
+  <si>
+    <t>floor</t>
+  </si>
+  <si>
+    <t>Cubes And Walled Offices</t>
+  </si>
+  <si>
+    <t>Americas/USBC/Building 1/Floor 2</t>
+  </si>
+  <si>
+    <t>Americas/USAU</t>
+  </si>
+  <si>
+    <t>Americas/USAU/Building 1</t>
+  </si>
+  <si>
+    <t>422 Somerset Rd., Winder, GA 30680</t>
+  </si>
+  <si>
+    <t>Americas/USAU/Building 1/Floor 1</t>
+  </si>
+  <si>
+    <t>Americas/USAU/Building 1/Floor 2</t>
+  </si>
+  <si>
+    <t>Americas/USBR</t>
+  </si>
+  <si>
+    <t>Americas/USBR/Building 1</t>
+  </si>
+  <si>
+    <t>1 Pine Ave., South Windsor, CT 06074</t>
+  </si>
+  <si>
+    <t>Americas/USBR/Building 1/Floor 1</t>
+  </si>
+  <si>
+    <t>Indoor High Ceiling</t>
+  </si>
+  <si>
+    <t>Americas/USBR/Building 2</t>
+  </si>
+  <si>
+    <t>Americas/USBR/Building 2/Floor 1</t>
+  </si>
+  <si>
+    <t>Drywall Office Only</t>
   </si>
 </sst>
 </file>
@@ -163,8 +214,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,9 +242,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,136 +562,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D82F1E7-4201-F546-8D7C-4F2671AD7BA9}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.5" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{461B1C34-C018-3443-9CDE-36DEFA6D593E}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -665,95 +870,95 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>